<commit_message>
CP Sheet introductory problems
</commit_message>
<xml_diff>
--- a/Codeforces/CP_SHEET.xlsx
+++ b/Codeforces/CP_SHEET.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
   <si>
     <t>Competitive Programming Sheet</t>
   </si>
@@ -31,6 +31,9 @@
     <t>Status</t>
   </si>
   <si>
+    <t>Number</t>
+  </si>
+  <si>
     <t>A</t>
   </si>
   <si>
@@ -44,6 +47,27 @@
   </si>
   <si>
     <t>https://codeforces.com/problemset/problem/263/A</t>
+  </si>
+  <si>
+    <t>Try Again</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/151/A</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/723/A</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/1352/A</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/510/A</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/785/A</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/144/A</t>
   </si>
 </sst>
 </file>
@@ -51,10 +75,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -104,6 +128,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -111,32 +157,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -148,24 +172,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -179,6 +195,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -187,51 +234,28 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,6 +276,72 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -264,7 +354,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -276,25 +372,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -306,19 +444,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,108 +475,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -443,6 +485,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -465,40 +531,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -535,6 +568,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -548,15 +590,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -569,131 +611,131 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -721,11 +763,32 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1046,10 +1109,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -1205,7 +1268,7 @@
       <c r="R8" s="3"/>
       <c r="S8" s="3"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:20">
       <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
@@ -1231,14 +1294,17 @@
       </c>
       <c r="R10" s="5"/>
       <c r="S10" s="5"/>
-    </row>
-    <row r="11" spans="1:19">
+      <c r="T10" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
       <c r="A11" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1254,18 +1320,21 @@
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
-    </row>
-    <row r="12" spans="1:19">
+      <c r="T11" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
       <c r="A12" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
@@ -1281,124 +1350,286 @@
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
       <c r="Q12" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="A13" s="6" t="s">
+      <c r="T12" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="17">
         <v>5</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="9" t="s">
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="17">
         <v>9</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="31">
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C10:P10"/>
     <mergeCell ref="Q10:S10"/>
@@ -1410,6 +1641,24 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="C13:P13"/>
     <mergeCell ref="Q13:S13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:P14"/>
+    <mergeCell ref="Q14:S14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:P15"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:P16"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:P17"/>
+    <mergeCell ref="Q17:S17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:P18"/>
+    <mergeCell ref="Q18:S18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:P19"/>
+    <mergeCell ref="Q19:S19"/>
     <mergeCell ref="A1:S5"/>
     <mergeCell ref="A7:S8"/>
   </mergeCells>
@@ -1417,6 +1666,12 @@
     <hyperlink ref="C11" r:id="rId1" display="https://codeforces.com/problemset/problem/282/A"/>
     <hyperlink ref="C12" r:id="rId2" display="https://codeforces.com/contest/514/problem/A"/>
     <hyperlink ref="C13" r:id="rId3" display="https://codeforces.com/problemset/problem/263/A"/>
+    <hyperlink ref="C14" r:id="rId4" display="https://codeforces.com/problemset/problem/151/A"/>
+    <hyperlink ref="C15" r:id="rId5" display="https://codeforces.com/problemset/problem/723/A"/>
+    <hyperlink ref="C16" r:id="rId6" display="https://codeforces.com/problemset/problem/1352/A"/>
+    <hyperlink ref="C17" r:id="rId7" display="https://codeforces.com/problemset/problem/510/A"/>
+    <hyperlink ref="C18" r:id="rId8" display="https://codeforces.com/problemset/problem/785/A"/>
+    <hyperlink ref="C19" r:id="rId9" display="https://codeforces.com/problemset/problem/144/A"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Contest round 771 problem a and b
</commit_message>
<xml_diff>
--- a/Codeforces/CP_SHEET.xlsx
+++ b/Codeforces/CP_SHEET.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$11:$B$39</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="43">
   <si>
     <t>Competitive Programming Sheet</t>
   </si>
@@ -46,6 +49,9 @@
     <t>https://codeforces.com/contest/514/problem/A</t>
   </si>
   <si>
+    <t>A - [IMP]</t>
+  </si>
+  <si>
     <t>https://codeforces.com/problemset/problem/263/A</t>
   </si>
   <si>
@@ -80,6 +86,66 @@
   </si>
   <si>
     <t>https://codeforces.com/problemset/problem/110/A</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/116/A</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/977/A</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/546/A</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/791/A</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/236/A</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/281/A</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/339/A</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/1368/A</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/702/A</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/1097/A</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/492/A</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/1433/A</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/1303/A</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/118/A</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/contest/1638/problem/A</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/1095/A</t>
+  </si>
+  <si>
+    <t>B - [V.IMP]</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/1391/B</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/1300/B</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -87,8 +153,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -139,8 +205,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -148,6 +229,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -163,6 +251,14 @@
     <font>
       <b/>
       <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -202,22 +298,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -231,7 +312,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -239,15 +320,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -259,15 +332,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,43 +342,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -324,13 +528,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -342,151 +546,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -497,6 +557,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -541,44 +616,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -597,12 +637,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -623,131 +683,131 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -775,6 +835,9 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -784,31 +847,13 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1130,10 +1175,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T60"/>
+  <dimension ref="A1:T62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:B23"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="Q45" sqref="Q45:S45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -1345,7 +1390,7 @@
       </c>
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
-      <c r="T11" s="20">
+      <c r="T11" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1375,37 +1420,37 @@
       </c>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
-      <c r="T12" s="20">
+      <c r="T12" s="15">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9" t="s">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="20">
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="15">
         <v>3</v>
       </c>
     </row>
@@ -1414,8 +1459,8 @@
         <v>6</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="11" t="s">
-        <v>12</v>
+      <c r="C14" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -1435,7 +1480,7 @@
       </c>
       <c r="R14" s="6"/>
       <c r="S14" s="6"/>
-      <c r="T14" s="20">
+      <c r="T14" s="15">
         <v>4</v>
       </c>
     </row>
@@ -1444,8 +1489,8 @@
         <v>6</v>
       </c>
       <c r="B15" s="6"/>
-      <c r="C15" s="11" t="s">
-        <v>13</v>
+      <c r="C15" s="12" t="s">
+        <v>14</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -1465,7 +1510,7 @@
       </c>
       <c r="R15" s="6"/>
       <c r="S15" s="6"/>
-      <c r="T15" s="20">
+      <c r="T15" s="15">
         <v>5</v>
       </c>
     </row>
@@ -1474,8 +1519,8 @@
         <v>6</v>
       </c>
       <c r="B16" s="6"/>
-      <c r="C16" s="11" t="s">
-        <v>14</v>
+      <c r="C16" s="12" t="s">
+        <v>15</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -1495,7 +1540,7 @@
       </c>
       <c r="R16" s="6"/>
       <c r="S16" s="6"/>
-      <c r="T16" s="20">
+      <c r="T16" s="15">
         <v>6</v>
       </c>
     </row>
@@ -1504,8 +1549,8 @@
         <v>6</v>
       </c>
       <c r="B17" s="6"/>
-      <c r="C17" s="11" t="s">
-        <v>15</v>
+      <c r="C17" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -1525,7 +1570,7 @@
       </c>
       <c r="R17" s="6"/>
       <c r="S17" s="6"/>
-      <c r="T17" s="20">
+      <c r="T17" s="15">
         <v>7</v>
       </c>
     </row>
@@ -1534,8 +1579,8 @@
         <v>6</v>
       </c>
       <c r="B18" s="6"/>
-      <c r="C18" s="11" t="s">
-        <v>16</v>
+      <c r="C18" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -1555,35 +1600,37 @@
       </c>
       <c r="R18" s="6"/>
       <c r="S18" s="6"/>
-      <c r="T18" s="20">
+      <c r="T18" s="15">
         <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:20">
-      <c r="A19" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="12"/>
-      <c r="S19" s="12"/>
-      <c r="T19" s="20">
+      <c r="A19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="15">
         <v>9</v>
       </c>
     </row>
@@ -1592,437 +1639,827 @@
         <v>6</v>
       </c>
       <c r="B20" s="6"/>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6"/>
+      <c r="T24" s="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="15">
         <v>18</v>
       </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15" t="s">
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="R20" s="15"/>
-      <c r="S20" s="15"/>
-      <c r="T20" s="20">
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="A31" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+      <c r="T31" s="15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="A32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R32" s="6"/>
+      <c r="S32" s="6"/>
+      <c r="T32" s="15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20">
+      <c r="A33" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R33" s="6"/>
+      <c r="S33" s="6"/>
+      <c r="T33" s="15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20">
+      <c r="A34" s="13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:20">
-      <c r="A21" s="6" t="s">
+      <c r="B34" s="6"/>
+      <c r="C34" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="R34" s="10"/>
+      <c r="S34" s="10"/>
+      <c r="T34" s="15">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20">
+      <c r="A35" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="10"/>
+      <c r="C35" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10"/>
+      <c r="T35" s="15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20">
+      <c r="A36" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="13"/>
+      <c r="C36" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="12"/>
+      <c r="P36" s="12"/>
+      <c r="Q36" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6"/>
+      <c r="T36" s="15">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20">
+      <c r="A37" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="12"/>
+      <c r="M37" s="12"/>
+      <c r="N37" s="12"/>
+      <c r="O37" s="12"/>
+      <c r="P37" s="12"/>
+      <c r="Q37" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="R37" s="10"/>
+      <c r="S37" s="10"/>
+      <c r="T37" s="15">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20">
+      <c r="A38" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="R21" s="17"/>
-      <c r="S21" s="17"/>
-      <c r="T21" s="20">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20">
-      <c r="A22" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
-      <c r="P22" s="17"/>
-      <c r="Q22" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="R22" s="17"/>
-      <c r="S22" s="17"/>
-      <c r="T22" s="20">
+      <c r="B38" s="6"/>
+      <c r="C38" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="6"/>
+      <c r="Q38" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R38" s="6"/>
+      <c r="S38" s="6"/>
+      <c r="T38" s="15">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20">
+      <c r="A39" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+      <c r="P39" s="6"/>
+      <c r="Q39" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R39" s="6"/>
+      <c r="S39" s="6"/>
+      <c r="T39" s="15">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20">
+      <c r="A40" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="10"/>
+      <c r="C40" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:20">
-      <c r="A23" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18"/>
-      <c r="T23" s="20">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18"/>
-      <c r="S24" s="18"/>
-      <c r="T24" s="20">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="Q25" s="18"/>
-      <c r="R25" s="18"/>
-      <c r="S25" s="18"/>
-      <c r="T25" s="20">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="18"/>
-      <c r="S26" s="18"/>
-      <c r="T26" s="20">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="Q27" s="18"/>
-      <c r="R27" s="18"/>
-      <c r="S27" s="18"/>
-      <c r="T27" s="20">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="Q28" s="18"/>
-      <c r="R28" s="18"/>
-      <c r="S28" s="18"/>
-      <c r="T28" s="20">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20">
-      <c r="A29" s="19"/>
-      <c r="B29" s="19"/>
-      <c r="Q29" s="18"/>
-      <c r="R29" s="18"/>
-      <c r="S29" s="18"/>
-      <c r="T29" s="20">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20">
-      <c r="A30" s="19"/>
-      <c r="B30" s="19"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="18"/>
-      <c r="S30" s="18"/>
-      <c r="T30" s="20">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20">
-      <c r="A31" s="19"/>
-      <c r="B31" s="19"/>
-      <c r="Q31" s="18"/>
-      <c r="R31" s="18"/>
-      <c r="S31" s="18"/>
-      <c r="T31" s="20">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20">
-      <c r="A32" s="19"/>
-      <c r="B32" s="19"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
-      <c r="S32" s="18"/>
-      <c r="T32" s="20">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20">
-      <c r="A33" s="19"/>
-      <c r="B33" s="19"/>
-      <c r="Q33" s="18"/>
-      <c r="R33" s="18"/>
-      <c r="S33" s="18"/>
-      <c r="T33" s="20">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20">
-      <c r="A34" s="19"/>
-      <c r="B34" s="19"/>
-      <c r="Q34" s="18"/>
-      <c r="R34" s="18"/>
-      <c r="S34" s="18"/>
-      <c r="T34" s="20">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="17:20">
-      <c r="Q35" s="18"/>
-      <c r="R35" s="18"/>
-      <c r="S35" s="18"/>
-      <c r="T35" s="20">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" spans="17:20">
-      <c r="Q36" s="18"/>
-      <c r="R36" s="18"/>
-      <c r="S36" s="18"/>
-      <c r="T36" s="20">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="17:20">
-      <c r="Q37" s="18"/>
-      <c r="R37" s="18"/>
-      <c r="S37" s="18"/>
-      <c r="T37" s="20">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="17:20">
-      <c r="Q38" s="18"/>
-      <c r="R38" s="18"/>
-      <c r="S38" s="18"/>
-      <c r="T38" s="20">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="39" spans="17:20">
-      <c r="Q39" s="18"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="18"/>
-      <c r="T39" s="20">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" spans="17:20">
-      <c r="Q40" s="18"/>
-      <c r="R40" s="18"/>
-      <c r="S40" s="18"/>
-      <c r="T40" s="20">
+      <c r="R40" s="10"/>
+      <c r="S40" s="10"/>
+      <c r="T40" s="15">
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="17:20">
-      <c r="Q41" s="18"/>
-      <c r="R41" s="18"/>
-      <c r="S41" s="18"/>
-      <c r="T41" s="20">
+    <row r="41" spans="1:20">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="3"/>
+      <c r="T41" s="15">
         <v>31</v>
       </c>
     </row>
     <row r="42" spans="17:20">
-      <c r="Q42" s="18"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="18"/>
-      <c r="T42" s="20">
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="3"/>
+      <c r="T42" s="15">
         <v>32</v>
       </c>
     </row>
     <row r="43" spans="17:20">
-      <c r="Q43" s="18"/>
-      <c r="R43" s="18"/>
-      <c r="S43" s="18"/>
-      <c r="T43" s="20">
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+      <c r="T43" s="15">
         <v>33</v>
       </c>
     </row>
     <row r="44" spans="17:20">
-      <c r="Q44" s="18"/>
-      <c r="R44" s="18"/>
-      <c r="S44" s="18"/>
-      <c r="T44" s="20">
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="3"/>
+      <c r="T44" s="15">
         <v>34</v>
       </c>
     </row>
     <row r="45" spans="17:20">
-      <c r="Q45" s="18"/>
-      <c r="R45" s="18"/>
-      <c r="S45" s="18"/>
-      <c r="T45" s="20">
+      <c r="Q45" s="3"/>
+      <c r="R45" s="3"/>
+      <c r="S45" s="3"/>
+      <c r="T45" s="15">
         <v>35</v>
       </c>
     </row>
     <row r="46" spans="17:20">
-      <c r="Q46" s="18"/>
-      <c r="R46" s="18"/>
-      <c r="S46" s="18"/>
-      <c r="T46" s="20">
+      <c r="Q46" s="3"/>
+      <c r="R46" s="3"/>
+      <c r="S46" s="3"/>
+      <c r="T46" s="15">
         <v>36</v>
       </c>
     </row>
     <row r="47" spans="17:20">
-      <c r="Q47" s="18"/>
-      <c r="R47" s="18"/>
-      <c r="S47" s="18"/>
-      <c r="T47" s="20">
+      <c r="Q47" s="3"/>
+      <c r="R47" s="3"/>
+      <c r="S47" s="3"/>
+      <c r="T47" s="15">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="17:20">
+      <c r="Q48" s="3"/>
+      <c r="R48" s="3"/>
+      <c r="S48" s="3"/>
+      <c r="T48" s="15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="17:20">
+      <c r="Q49" s="3"/>
+      <c r="R49" s="3"/>
+      <c r="S49" s="3"/>
+      <c r="T49" s="15">
         <v>37</v>
       </c>
     </row>
-    <row r="48" spans="17:20">
-      <c r="Q48" s="18"/>
-      <c r="R48" s="18"/>
-      <c r="S48" s="18"/>
-      <c r="T48" s="20">
+    <row r="50" spans="17:20">
+      <c r="Q50" s="3"/>
+      <c r="R50" s="3"/>
+      <c r="S50" s="3"/>
+      <c r="T50" s="15">
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="17:20">
-      <c r="Q49" s="18"/>
-      <c r="R49" s="18"/>
-      <c r="S49" s="18"/>
-      <c r="T49" s="20">
+    <row r="51" spans="17:20">
+      <c r="Q51" s="3"/>
+      <c r="R51" s="3"/>
+      <c r="S51" s="3"/>
+      <c r="T51" s="15">
         <v>39</v>
       </c>
     </row>
-    <row r="50" spans="17:20">
-      <c r="Q50" s="18"/>
-      <c r="R50" s="18"/>
-      <c r="S50" s="18"/>
-      <c r="T50" s="20">
+    <row r="52" spans="17:20">
+      <c r="Q52" s="3"/>
+      <c r="R52" s="3"/>
+      <c r="S52" s="3"/>
+      <c r="T52" s="15">
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="17:20">
-      <c r="Q51" s="18"/>
-      <c r="R51" s="18"/>
-      <c r="S51" s="18"/>
-      <c r="T51" s="20">
+    <row r="53" spans="17:20">
+      <c r="Q53" s="3"/>
+      <c r="R53" s="3"/>
+      <c r="S53" s="3"/>
+      <c r="T53" s="15">
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="17:20">
-      <c r="Q52" s="18"/>
-      <c r="R52" s="18"/>
-      <c r="S52" s="18"/>
-      <c r="T52" s="20">
+    <row r="54" spans="17:20">
+      <c r="Q54" s="3"/>
+      <c r="R54" s="3"/>
+      <c r="S54" s="3"/>
+      <c r="T54" s="15">
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="17:20">
-      <c r="Q53" s="18"/>
-      <c r="R53" s="18"/>
-      <c r="S53" s="18"/>
-      <c r="T53" s="20">
+    <row r="55" spans="17:20">
+      <c r="Q55" s="3"/>
+      <c r="R55" s="3"/>
+      <c r="S55" s="3"/>
+      <c r="T55" s="15">
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="17:20">
-      <c r="Q54" s="18"/>
-      <c r="R54" s="18"/>
-      <c r="S54" s="18"/>
-      <c r="T54" s="20">
+    <row r="56" spans="17:20">
+      <c r="Q56" s="3"/>
+      <c r="R56" s="3"/>
+      <c r="S56" s="3"/>
+      <c r="T56" s="15">
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="17:20">
-      <c r="Q55" s="18"/>
-      <c r="R55" s="18"/>
-      <c r="S55" s="18"/>
-      <c r="T55" s="20">
+    <row r="57" spans="17:20">
+      <c r="Q57" s="3"/>
+      <c r="R57" s="3"/>
+      <c r="S57" s="3"/>
+      <c r="T57" s="15">
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="17:20">
-      <c r="Q56" s="18"/>
-      <c r="R56" s="18"/>
-      <c r="S56" s="18"/>
-      <c r="T56" s="20">
+    <row r="58" spans="17:20">
+      <c r="Q58" s="3"/>
+      <c r="R58" s="3"/>
+      <c r="S58" s="3"/>
+      <c r="T58" s="15">
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="17:20">
-      <c r="Q57" s="18"/>
-      <c r="R57" s="18"/>
-      <c r="S57" s="18"/>
-      <c r="T57" s="20">
+    <row r="59" spans="17:20">
+      <c r="Q59" s="3"/>
+      <c r="R59" s="3"/>
+      <c r="S59" s="3"/>
+      <c r="T59" s="15">
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="17:20">
-      <c r="Q58" s="18"/>
-      <c r="R58" s="18"/>
-      <c r="S58" s="18"/>
-      <c r="T58" s="20">
+    <row r="60" spans="17:20">
+      <c r="Q60" s="3"/>
+      <c r="R60" s="3"/>
+      <c r="S60" s="3"/>
+      <c r="T60" s="15">
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="17:20">
-      <c r="Q59" s="18"/>
-      <c r="R59" s="18"/>
-      <c r="S59" s="18"/>
-      <c r="T59" s="20">
+    <row r="61" spans="17:20">
+      <c r="Q61" s="3"/>
+      <c r="R61" s="3"/>
+      <c r="S61" s="3"/>
+      <c r="T61" s="15">
         <v>49</v>
       </c>
     </row>
-    <row r="60" spans="17:20">
-      <c r="Q60" s="18"/>
-      <c r="R60" s="18"/>
-      <c r="S60" s="18"/>
-      <c r="T60" s="20">
+    <row r="62" spans="17:20">
+      <c r="Q62" s="3"/>
+      <c r="R62" s="3"/>
+      <c r="S62" s="3"/>
+      <c r="T62" s="15">
         <v>50</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="85">
+  <mergeCells count="118">
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C10:P10"/>
     <mergeCell ref="Q10:S10"/>
@@ -2065,27 +2502,58 @@
     <mergeCell ref="C23:P23"/>
     <mergeCell ref="Q23:S23"/>
     <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:P24"/>
     <mergeCell ref="Q24:S24"/>
     <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:P25"/>
     <mergeCell ref="Q25:S25"/>
     <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:P26"/>
     <mergeCell ref="Q26:S26"/>
     <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:P27"/>
     <mergeCell ref="Q27:S27"/>
     <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:P28"/>
     <mergeCell ref="Q28:S28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:P29"/>
     <mergeCell ref="Q29:S29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:P30"/>
     <mergeCell ref="Q30:S30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:P31"/>
     <mergeCell ref="Q31:S31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:P32"/>
     <mergeCell ref="Q32:S32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:P33"/>
     <mergeCell ref="Q33:S33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:P34"/>
     <mergeCell ref="Q34:S34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:P35"/>
     <mergeCell ref="Q35:S35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C36:P36"/>
     <mergeCell ref="Q36:S36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:P37"/>
     <mergeCell ref="Q37:S37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:P38"/>
     <mergeCell ref="Q38:S38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:P39"/>
     <mergeCell ref="Q39:S39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:P40"/>
     <mergeCell ref="Q40:S40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:P41"/>
     <mergeCell ref="Q41:S41"/>
     <mergeCell ref="Q42:S42"/>
     <mergeCell ref="Q43:S43"/>
@@ -2106,6 +2574,8 @@
     <mergeCell ref="Q58:S58"/>
     <mergeCell ref="Q59:S59"/>
     <mergeCell ref="Q60:S60"/>
+    <mergeCell ref="Q61:S61"/>
+    <mergeCell ref="Q62:S62"/>
     <mergeCell ref="A1:S5"/>
     <mergeCell ref="A7:S8"/>
   </mergeCells>
@@ -2121,7 +2591,25 @@
     <hyperlink ref="C19" r:id="rId9" display="https://codeforces.com/problemset/problem/144/A"/>
     <hyperlink ref="C20" r:id="rId10" display="https://codeforces.com/problemset/problem/1030/A"/>
     <hyperlink ref="C21" r:id="rId11" display="https://codeforces.com/problemset/problem/136/A"/>
-    <hyperlink ref="C22" r:id="rId12" display="https://codeforces.com/problemset/problem/110/A"/>
+    <hyperlink ref="C22" r:id="rId12" display="https://codeforces.com/problemset/problem/110/A" tooltip="https://codeforces.com/problemset/problem/110/A"/>
+    <hyperlink ref="C23" r:id="rId13" display="https://codeforces.com/problemset/problem/116/A"/>
+    <hyperlink ref="C24" r:id="rId14" display="https://codeforces.com/problemset/problem/977/A"/>
+    <hyperlink ref="C25" r:id="rId15" display="https://codeforces.com/problemset/problem/546/A"/>
+    <hyperlink ref="C26" r:id="rId16" display="https://codeforces.com/problemset/problem/791/A"/>
+    <hyperlink ref="C27" r:id="rId17" display="https://codeforces.com/problemset/problem/236/A"/>
+    <hyperlink ref="C28" r:id="rId18" display="https://codeforces.com/problemset/problem/281/A"/>
+    <hyperlink ref="C29" r:id="rId19" display="https://codeforces.com/problemset/problem/339/A"/>
+    <hyperlink ref="C30" r:id="rId20" display="https://codeforces.com/problemset/problem/1368/A"/>
+    <hyperlink ref="C31" r:id="rId21" display="https://codeforces.com/problemset/problem/702/A"/>
+    <hyperlink ref="C32" r:id="rId22" display="https://codeforces.com/problemset/problem/1097/A"/>
+    <hyperlink ref="C33" r:id="rId23" display="https://codeforces.com/problemset/problem/492/A"/>
+    <hyperlink ref="C34" r:id="rId24" display="https://codeforces.com/problemset/problem/1433/A"/>
+    <hyperlink ref="C35" r:id="rId25" display="https://codeforces.com/problemset/problem/1303/A"/>
+    <hyperlink ref="C38" r:id="rId26" display="https://codeforces.com/problemset/problem/1095/A"/>
+    <hyperlink ref="C39" r:id="rId27" display="https://codeforces.com/problemset/problem/1391/B"/>
+    <hyperlink ref="C36" r:id="rId28" display="https://codeforces.com/problemset/problem/118/A"/>
+    <hyperlink ref="C40" r:id="rId29" display="https://codeforces.com/problemset/problem/1300/B"/>
+    <hyperlink ref="C37" r:id="rId30" display="https://codeforces.com/contest/1638/problem/A"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
DSA - day 2
</commit_message>
<xml_diff>
--- a/Codeforces/CP_SHEET.xlsx
+++ b/Codeforces/CP_SHEET.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$11:$B$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$11:$B$40</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
   <si>
     <t>Competitive Programming Sheet</t>
   </si>
@@ -133,10 +133,13 @@
     <t>https://codeforces.com/contest/1638/problem/A</t>
   </si>
   <si>
+    <t>https://codeforces.com/contest/139/problem/A</t>
+  </si>
+  <si>
     <t>https://codeforces.com/problemset/problem/1095/A</t>
   </si>
   <si>
-    <t>B - [V.IMP]</t>
+    <t>B - [IMP]</t>
   </si>
   <si>
     <t>https://codeforces.com/problemset/problem/1391/B</t>
@@ -145,7 +148,13 @@
     <t>https://codeforces.com/problemset/problem/1300/B</t>
   </si>
   <si>
-    <t>s</t>
+    <t>https://codeforces.com/contest/1638/problem/B</t>
+  </si>
+  <si>
+    <t>C - [IMP]</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/1430/C</t>
   </si>
 </sst>
 </file>
@@ -153,10 +162,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -205,9 +214,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -221,19 +265,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -254,21 +292,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -296,6 +319,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -304,34 +334,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="37">
     <fill>
@@ -366,19 +375,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -390,7 +525,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -402,97 +537,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -504,49 +555,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -560,17 +569,31 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -614,11 +637,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -637,26 +666,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -665,12 +674,12 @@
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -683,127 +692,127 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1175,10 +1184,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T62"/>
+  <dimension ref="A1:T65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="Q45" sqref="Q45:S45"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="Q62" sqref="Q62:S62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -2175,26 +2184,26 @@
       </c>
     </row>
     <row r="38" spans="1:20">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="6"/>
+      <c r="B38" s="13"/>
       <c r="C38" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
+      <c r="N38" s="12"/>
+      <c r="O38" s="12"/>
+      <c r="P38" s="12"/>
       <c r="Q38" s="6" t="s">
         <v>8</v>
       </c>
@@ -2205,12 +2214,12 @@
       </c>
     </row>
     <row r="39" spans="1:20">
-      <c r="A39" s="13" t="s">
-        <v>39</v>
+      <c r="A39" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -2235,78 +2244,128 @@
       </c>
     </row>
     <row r="40" spans="1:20">
-      <c r="A40" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B40" s="10"/>
-      <c r="C40" s="11" t="s">
+      <c r="A40" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="6"/>
+      <c r="C40" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="10"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="10"/>
-      <c r="K40" s="10"/>
-      <c r="L40" s="10"/>
-      <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
-      <c r="O40" s="10"/>
-      <c r="P40" s="10"/>
-      <c r="Q40" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="R40" s="10"/>
-      <c r="S40" s="10"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="6"/>
+      <c r="Q40" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R40" s="6"/>
+      <c r="S40" s="6"/>
       <c r="T40" s="15">
         <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:20">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3" t="s">
+      <c r="A41" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="10"/>
+      <c r="C41" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
-      <c r="O41" s="3"/>
-      <c r="P41" s="3"/>
-      <c r="Q41" s="3"/>
-      <c r="R41" s="3"/>
-      <c r="S41" s="3"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="10"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="10"/>
+      <c r="Q41" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R41" s="10"/>
+      <c r="S41" s="10"/>
       <c r="T41" s="15">
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="17:20">
-      <c r="Q42" s="3"/>
-      <c r="R42" s="3"/>
-      <c r="S42" s="3"/>
+    <row r="42" spans="1:20">
+      <c r="A42" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="6"/>
+      <c r="C42" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
+      <c r="P42" s="6"/>
+      <c r="Q42" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="R42" s="10"/>
+      <c r="S42" s="10"/>
       <c r="T42" s="15">
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="17:20">
-      <c r="Q43" s="3"/>
-      <c r="R43" s="3"/>
-      <c r="S43" s="3"/>
+    <row r="43" spans="1:20">
+      <c r="A43" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="6"/>
+      <c r="P43" s="6"/>
+      <c r="Q43" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R43" s="6"/>
+      <c r="S43" s="6"/>
       <c r="T43" s="15">
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="17:20">
+    <row r="44" spans="1:20">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
       <c r="Q44" s="3"/>
       <c r="R44" s="3"/>
       <c r="S44" s="3"/>
@@ -2314,7 +2373,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="17:20">
+    <row r="45" spans="1:20">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
       <c r="Q45" s="3"/>
       <c r="R45" s="3"/>
       <c r="S45" s="3"/>
@@ -2322,7 +2383,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="17:20">
+    <row r="46" spans="1:20">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
       <c r="Q46" s="3"/>
       <c r="R46" s="3"/>
       <c r="S46" s="3"/>
@@ -2330,60 +2393,74 @@
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="17:20">
+    <row r="47" spans="1:20">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
       <c r="Q47" s="3"/>
       <c r="R47" s="3"/>
       <c r="S47" s="3"/>
       <c r="T47" s="15">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="48" spans="17:20">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
       <c r="Q48" s="3"/>
       <c r="R48" s="3"/>
       <c r="S48" s="3"/>
       <c r="T48" s="15">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="49" spans="17:20">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
       <c r="Q49" s="3"/>
       <c r="R49" s="3"/>
       <c r="S49" s="3"/>
       <c r="T49" s="15">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="50" spans="17:20">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
       <c r="Q50" s="3"/>
       <c r="R50" s="3"/>
       <c r="S50" s="3"/>
       <c r="T50" s="15">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="51" spans="17:20">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
       <c r="Q51" s="3"/>
       <c r="R51" s="3"/>
       <c r="S51" s="3"/>
       <c r="T51" s="15">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="52" spans="17:20">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
       <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
       <c r="S52" s="3"/>
       <c r="T52" s="15">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="53" spans="17:20">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
       <c r="Q53" s="3"/>
       <c r="R53" s="3"/>
       <c r="S53" s="3"/>
       <c r="T53" s="15">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="17:20">
@@ -2391,7 +2468,7 @@
       <c r="R54" s="3"/>
       <c r="S54" s="3"/>
       <c r="T54" s="15">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="17:20">
@@ -2399,7 +2476,7 @@
       <c r="R55" s="3"/>
       <c r="S55" s="3"/>
       <c r="T55" s="15">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="17:20">
@@ -2407,7 +2484,7 @@
       <c r="R56" s="3"/>
       <c r="S56" s="3"/>
       <c r="T56" s="15">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="57" spans="17:20">
@@ -2415,7 +2492,7 @@
       <c r="R57" s="3"/>
       <c r="S57" s="3"/>
       <c r="T57" s="15">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="58" spans="17:20">
@@ -2423,7 +2500,7 @@
       <c r="R58" s="3"/>
       <c r="S58" s="3"/>
       <c r="T58" s="15">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="59" spans="17:20">
@@ -2431,7 +2508,7 @@
       <c r="R59" s="3"/>
       <c r="S59" s="3"/>
       <c r="T59" s="15">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="60" spans="17:20">
@@ -2439,7 +2516,7 @@
       <c r="R60" s="3"/>
       <c r="S60" s="3"/>
       <c r="T60" s="15">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="61" spans="17:20">
@@ -2447,7 +2524,7 @@
       <c r="R61" s="3"/>
       <c r="S61" s="3"/>
       <c r="T61" s="15">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="62" spans="17:20">
@@ -2455,11 +2532,29 @@
       <c r="R62" s="3"/>
       <c r="S62" s="3"/>
       <c r="T62" s="15">
-        <v>50</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="63" spans="17:20">
+      <c r="Q63" s="3"/>
+      <c r="R63" s="3"/>
+      <c r="S63" s="3"/>
+      <c r="T63" s="15">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="20:20">
+      <c r="T64" s="15">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="20:20">
+      <c r="T65" s="15">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="118">
+  <mergeCells count="133">
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C10:P10"/>
     <mergeCell ref="Q10:S10"/>
@@ -2555,17 +2650,31 @@
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="C41:P41"/>
     <mergeCell ref="Q41:S41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:P42"/>
     <mergeCell ref="Q42:S42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:P43"/>
     <mergeCell ref="Q43:S43"/>
+    <mergeCell ref="A44:B44"/>
     <mergeCell ref="Q44:S44"/>
+    <mergeCell ref="A45:B45"/>
     <mergeCell ref="Q45:S45"/>
+    <mergeCell ref="A46:B46"/>
     <mergeCell ref="Q46:S46"/>
+    <mergeCell ref="A47:B47"/>
     <mergeCell ref="Q47:S47"/>
+    <mergeCell ref="A48:B48"/>
     <mergeCell ref="Q48:S48"/>
+    <mergeCell ref="A49:B49"/>
     <mergeCell ref="Q49:S49"/>
+    <mergeCell ref="A50:B50"/>
     <mergeCell ref="Q50:S50"/>
+    <mergeCell ref="A51:B51"/>
     <mergeCell ref="Q51:S51"/>
+    <mergeCell ref="A52:B52"/>
     <mergeCell ref="Q52:S52"/>
+    <mergeCell ref="A53:B53"/>
     <mergeCell ref="Q53:S53"/>
     <mergeCell ref="Q54:S54"/>
     <mergeCell ref="Q55:S55"/>
@@ -2576,6 +2685,7 @@
     <mergeCell ref="Q60:S60"/>
     <mergeCell ref="Q61:S61"/>
     <mergeCell ref="Q62:S62"/>
+    <mergeCell ref="Q63:S63"/>
     <mergeCell ref="A1:S5"/>
     <mergeCell ref="A7:S8"/>
   </mergeCells>
@@ -2605,11 +2715,14 @@
     <hyperlink ref="C33" r:id="rId23" display="https://codeforces.com/problemset/problem/492/A"/>
     <hyperlink ref="C34" r:id="rId24" display="https://codeforces.com/problemset/problem/1433/A"/>
     <hyperlink ref="C35" r:id="rId25" display="https://codeforces.com/problemset/problem/1303/A"/>
-    <hyperlink ref="C38" r:id="rId26" display="https://codeforces.com/problemset/problem/1095/A"/>
-    <hyperlink ref="C39" r:id="rId27" display="https://codeforces.com/problemset/problem/1391/B"/>
+    <hyperlink ref="C39" r:id="rId26" display="https://codeforces.com/problemset/problem/1095/A"/>
+    <hyperlink ref="C40" r:id="rId27" display="https://codeforces.com/problemset/problem/1391/B"/>
     <hyperlink ref="C36" r:id="rId28" display="https://codeforces.com/problemset/problem/118/A"/>
-    <hyperlink ref="C40" r:id="rId29" display="https://codeforces.com/problemset/problem/1300/B"/>
+    <hyperlink ref="C41" r:id="rId29" display="https://codeforces.com/problemset/problem/1300/B"/>
     <hyperlink ref="C37" r:id="rId30" display="https://codeforces.com/contest/1638/problem/A"/>
+    <hyperlink ref="C42" r:id="rId31" display="https://codeforces.com/contest/1638/problem/B"/>
+    <hyperlink ref="C43" r:id="rId32" display="https://codeforces.com/problemset/problem/1430/C"/>
+    <hyperlink ref="C38" r:id="rId33" display="https://codeforces.com/contest/139/problem/A"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Dsa day4 queue question
</commit_message>
<xml_diff>
--- a/Codeforces/CP_SHEET.xlsx
+++ b/Codeforces/CP_SHEET.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="50">
   <si>
     <t>Competitive Programming Sheet</t>
   </si>
@@ -155,6 +155,18 @@
   </si>
   <si>
     <t>https://codeforces.com/problemset/problem/1430/C</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/219/A</t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/1141/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B </t>
+  </si>
+  <si>
+    <t>https://codeforces.com/problemset/problem/118/B</t>
   </si>
 </sst>
 </file>
@@ -162,10 +174,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -215,29 +227,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -251,13 +248,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -265,15 +255,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -319,8 +301,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -333,14 +353,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="37">
     <fill>
@@ -375,187 +387,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -566,35 +578,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -637,6 +620,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -648,6 +651,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -671,15 +683,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -692,131 +704,131 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -860,6 +872,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1186,8 +1210,8 @@
   <sheetPr/>
   <dimension ref="A1:T65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="Q62" sqref="Q62:S62"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48:B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -1399,7 +1423,7 @@
       </c>
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
-      <c r="T11" s="15">
+      <c r="T11" s="19">
         <v>1</v>
       </c>
     </row>
@@ -1429,7 +1453,7 @@
       </c>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
-      <c r="T12" s="15">
+      <c r="T12" s="19">
         <v>2</v>
       </c>
     </row>
@@ -1459,7 +1483,7 @@
       </c>
       <c r="R13" s="10"/>
       <c r="S13" s="10"/>
-      <c r="T13" s="15">
+      <c r="T13" s="19">
         <v>3</v>
       </c>
     </row>
@@ -1489,7 +1513,7 @@
       </c>
       <c r="R14" s="6"/>
       <c r="S14" s="6"/>
-      <c r="T14" s="15">
+      <c r="T14" s="19">
         <v>4</v>
       </c>
     </row>
@@ -1519,7 +1543,7 @@
       </c>
       <c r="R15" s="6"/>
       <c r="S15" s="6"/>
-      <c r="T15" s="15">
+      <c r="T15" s="19">
         <v>5</v>
       </c>
     </row>
@@ -1549,7 +1573,7 @@
       </c>
       <c r="R16" s="6"/>
       <c r="S16" s="6"/>
-      <c r="T16" s="15">
+      <c r="T16" s="19">
         <v>6</v>
       </c>
     </row>
@@ -1579,7 +1603,7 @@
       </c>
       <c r="R17" s="6"/>
       <c r="S17" s="6"/>
-      <c r="T17" s="15">
+      <c r="T17" s="19">
         <v>7</v>
       </c>
     </row>
@@ -1609,7 +1633,7 @@
       </c>
       <c r="R18" s="6"/>
       <c r="S18" s="6"/>
-      <c r="T18" s="15">
+      <c r="T18" s="19">
         <v>8</v>
       </c>
     </row>
@@ -1639,7 +1663,7 @@
       </c>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
-      <c r="T19" s="15">
+      <c r="T19" s="19">
         <v>9</v>
       </c>
     </row>
@@ -1669,7 +1693,7 @@
       </c>
       <c r="R20" s="6"/>
       <c r="S20" s="6"/>
-      <c r="T20" s="15">
+      <c r="T20" s="19">
         <v>10</v>
       </c>
     </row>
@@ -1699,7 +1723,7 @@
       </c>
       <c r="R21" s="10"/>
       <c r="S21" s="10"/>
-      <c r="T21" s="15">
+      <c r="T21" s="19">
         <v>11</v>
       </c>
     </row>
@@ -1729,7 +1753,7 @@
       </c>
       <c r="R22" s="10"/>
       <c r="S22" s="10"/>
-      <c r="T22" s="15">
+      <c r="T22" s="19">
         <v>12</v>
       </c>
     </row>
@@ -1759,7 +1783,7 @@
       </c>
       <c r="R23" s="6"/>
       <c r="S23" s="6"/>
-      <c r="T23" s="15">
+      <c r="T23" s="19">
         <v>13</v>
       </c>
     </row>
@@ -1789,7 +1813,7 @@
       </c>
       <c r="R24" s="6"/>
       <c r="S24" s="6"/>
-      <c r="T24" s="15">
+      <c r="T24" s="19">
         <v>14</v>
       </c>
     </row>
@@ -1819,7 +1843,7 @@
       </c>
       <c r="R25" s="6"/>
       <c r="S25" s="6"/>
-      <c r="T25" s="15">
+      <c r="T25" s="19">
         <v>15</v>
       </c>
     </row>
@@ -1849,7 +1873,7 @@
       </c>
       <c r="R26" s="6"/>
       <c r="S26" s="6"/>
-      <c r="T26" s="15">
+      <c r="T26" s="19">
         <v>16</v>
       </c>
     </row>
@@ -1879,7 +1903,7 @@
       </c>
       <c r="R27" s="6"/>
       <c r="S27" s="6"/>
-      <c r="T27" s="15">
+      <c r="T27" s="19">
         <v>17</v>
       </c>
     </row>
@@ -1909,7 +1933,7 @@
       </c>
       <c r="R28" s="6"/>
       <c r="S28" s="6"/>
-      <c r="T28" s="15">
+      <c r="T28" s="19">
         <v>18</v>
       </c>
     </row>
@@ -1939,7 +1963,7 @@
       </c>
       <c r="R29" s="6"/>
       <c r="S29" s="6"/>
-      <c r="T29" s="15">
+      <c r="T29" s="19">
         <v>19</v>
       </c>
     </row>
@@ -1969,7 +1993,7 @@
       </c>
       <c r="R30" s="6"/>
       <c r="S30" s="6"/>
-      <c r="T30" s="15">
+      <c r="T30" s="19">
         <v>20</v>
       </c>
     </row>
@@ -1999,7 +2023,7 @@
       </c>
       <c r="R31" s="6"/>
       <c r="S31" s="6"/>
-      <c r="T31" s="15">
+      <c r="T31" s="19">
         <v>21</v>
       </c>
     </row>
@@ -2029,7 +2053,7 @@
       </c>
       <c r="R32" s="6"/>
       <c r="S32" s="6"/>
-      <c r="T32" s="15">
+      <c r="T32" s="19">
         <v>22</v>
       </c>
     </row>
@@ -2059,7 +2083,7 @@
       </c>
       <c r="R33" s="6"/>
       <c r="S33" s="6"/>
-      <c r="T33" s="15">
+      <c r="T33" s="19">
         <v>23</v>
       </c>
     </row>
@@ -2089,7 +2113,7 @@
       </c>
       <c r="R34" s="10"/>
       <c r="S34" s="10"/>
-      <c r="T34" s="15">
+      <c r="T34" s="19">
         <v>24</v>
       </c>
     </row>
@@ -2119,7 +2143,7 @@
       </c>
       <c r="R35" s="10"/>
       <c r="S35" s="10"/>
-      <c r="T35" s="15">
+      <c r="T35" s="19">
         <v>25</v>
       </c>
     </row>
@@ -2149,7 +2173,7 @@
       </c>
       <c r="R36" s="6"/>
       <c r="S36" s="6"/>
-      <c r="T36" s="15">
+      <c r="T36" s="19">
         <v>26</v>
       </c>
     </row>
@@ -2179,7 +2203,7 @@
       </c>
       <c r="R37" s="10"/>
       <c r="S37" s="10"/>
-      <c r="T37" s="15">
+      <c r="T37" s="19">
         <v>27</v>
       </c>
     </row>
@@ -2209,7 +2233,7 @@
       </c>
       <c r="R38" s="6"/>
       <c r="S38" s="6"/>
-      <c r="T38" s="15">
+      <c r="T38" s="19">
         <v>28</v>
       </c>
     </row>
@@ -2239,7 +2263,7 @@
       </c>
       <c r="R39" s="6"/>
       <c r="S39" s="6"/>
-      <c r="T39" s="15">
+      <c r="T39" s="19">
         <v>29</v>
       </c>
     </row>
@@ -2269,7 +2293,7 @@
       </c>
       <c r="R40" s="6"/>
       <c r="S40" s="6"/>
-      <c r="T40" s="15">
+      <c r="T40" s="19">
         <v>30</v>
       </c>
     </row>
@@ -2299,7 +2323,7 @@
       </c>
       <c r="R41" s="10"/>
       <c r="S41" s="10"/>
-      <c r="T41" s="15">
+      <c r="T41" s="19">
         <v>31</v>
       </c>
     </row>
@@ -2329,7 +2353,7 @@
       </c>
       <c r="R42" s="10"/>
       <c r="S42" s="10"/>
-      <c r="T42" s="15">
+      <c r="T42" s="19">
         <v>32</v>
       </c>
     </row>
@@ -2359,202 +2383,562 @@
       </c>
       <c r="R43" s="6"/>
       <c r="S43" s="6"/>
-      <c r="T43" s="15">
+      <c r="T43" s="19">
         <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:20">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="Q44" s="3"/>
-      <c r="R44" s="3"/>
-      <c r="S44" s="3"/>
-      <c r="T44" s="15">
+      <c r="A44" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="6"/>
+      <c r="C44" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="15"/>
+      <c r="L44" s="15"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R44" s="6"/>
+      <c r="S44" s="6"/>
+      <c r="T44" s="19">
         <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:20">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="Q45" s="3"/>
-      <c r="R45" s="3"/>
-      <c r="S45" s="3"/>
-      <c r="T45" s="15">
+      <c r="A45" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="10"/>
+      <c r="C45" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="16"/>
+      <c r="L45" s="16"/>
+      <c r="M45" s="16"/>
+      <c r="N45" s="16"/>
+      <c r="O45" s="16"/>
+      <c r="P45" s="16"/>
+      <c r="Q45" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R45" s="10"/>
+      <c r="S45" s="10"/>
+      <c r="T45" s="19">
         <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:20">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="Q46" s="3"/>
-      <c r="R46" s="3"/>
-      <c r="S46" s="3"/>
-      <c r="T46" s="15">
+      <c r="A46" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="6"/>
+      <c r="C46" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="15"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="15"/>
+      <c r="O46" s="15"/>
+      <c r="P46" s="15"/>
+      <c r="Q46" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="R46" s="6"/>
+      <c r="S46" s="6"/>
+      <c r="T46" s="19">
         <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:20">
-      <c r="A47" s="3"/>
+      <c r="A47" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="B47" s="3"/>
+      <c r="C47" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="17"/>
+      <c r="L47" s="17"/>
+      <c r="M47" s="17"/>
+      <c r="N47" s="17"/>
+      <c r="O47" s="17"/>
+      <c r="P47" s="17"/>
       <c r="Q47" s="3"/>
       <c r="R47" s="3"/>
       <c r="S47" s="3"/>
-      <c r="T47" s="15">
+      <c r="T47" s="19">
         <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:20">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="18"/>
+      <c r="N48" s="18"/>
+      <c r="O48" s="18"/>
+      <c r="P48" s="18"/>
       <c r="Q48" s="3"/>
       <c r="R48" s="3"/>
       <c r="S48" s="3"/>
-      <c r="T48" s="15">
+      <c r="T48" s="19">
         <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:20">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="18"/>
+      <c r="M49" s="18"/>
+      <c r="N49" s="18"/>
+      <c r="O49" s="18"/>
+      <c r="P49" s="18"/>
       <c r="Q49" s="3"/>
       <c r="R49" s="3"/>
       <c r="S49" s="3"/>
-      <c r="T49" s="15">
+      <c r="T49" s="19">
         <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:20">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="18"/>
+      <c r="M50" s="18"/>
+      <c r="N50" s="18"/>
+      <c r="O50" s="18"/>
+      <c r="P50" s="18"/>
       <c r="Q50" s="3"/>
       <c r="R50" s="3"/>
       <c r="S50" s="3"/>
-      <c r="T50" s="15">
+      <c r="T50" s="19">
         <v>40</v>
       </c>
     </row>
     <row r="51" spans="1:20">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="18"/>
+      <c r="K51" s="18"/>
+      <c r="L51" s="18"/>
+      <c r="M51" s="18"/>
+      <c r="N51" s="18"/>
+      <c r="O51" s="18"/>
+      <c r="P51" s="18"/>
       <c r="Q51" s="3"/>
       <c r="R51" s="3"/>
       <c r="S51" s="3"/>
-      <c r="T51" s="15">
+      <c r="T51" s="19">
         <v>41</v>
       </c>
     </row>
     <row r="52" spans="1:20">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="18"/>
+      <c r="K52" s="18"/>
+      <c r="L52" s="18"/>
+      <c r="M52" s="18"/>
+      <c r="N52" s="18"/>
+      <c r="O52" s="18"/>
+      <c r="P52" s="18"/>
       <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
       <c r="S52" s="3"/>
-      <c r="T52" s="15">
+      <c r="T52" s="19">
         <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:20">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="18"/>
+      <c r="N53" s="18"/>
+      <c r="O53" s="18"/>
+      <c r="P53" s="18"/>
       <c r="Q53" s="3"/>
       <c r="R53" s="3"/>
       <c r="S53" s="3"/>
-      <c r="T53" s="15">
+      <c r="T53" s="19">
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="17:20">
+    <row r="54" spans="1:20">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+      <c r="I54" s="18"/>
+      <c r="J54" s="18"/>
+      <c r="K54" s="18"/>
+      <c r="L54" s="18"/>
+      <c r="M54" s="18"/>
+      <c r="N54" s="18"/>
+      <c r="O54" s="18"/>
+      <c r="P54" s="18"/>
       <c r="Q54" s="3"/>
       <c r="R54" s="3"/>
       <c r="S54" s="3"/>
-      <c r="T54" s="15">
+      <c r="T54" s="19">
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="17:20">
+    <row r="55" spans="1:20">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="18"/>
+      <c r="J55" s="18"/>
+      <c r="K55" s="18"/>
+      <c r="L55" s="18"/>
+      <c r="M55" s="18"/>
+      <c r="N55" s="18"/>
+      <c r="O55" s="18"/>
+      <c r="P55" s="18"/>
       <c r="Q55" s="3"/>
       <c r="R55" s="3"/>
       <c r="S55" s="3"/>
-      <c r="T55" s="15">
+      <c r="T55" s="19">
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="17:20">
+    <row r="56" spans="1:20">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+      <c r="I56" s="18"/>
+      <c r="J56" s="18"/>
+      <c r="K56" s="18"/>
+      <c r="L56" s="18"/>
+      <c r="M56" s="18"/>
+      <c r="N56" s="18"/>
+      <c r="O56" s="18"/>
+      <c r="P56" s="18"/>
       <c r="Q56" s="3"/>
       <c r="R56" s="3"/>
       <c r="S56" s="3"/>
-      <c r="T56" s="15">
+      <c r="T56" s="19">
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="17:20">
+    <row r="57" spans="1:20">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+      <c r="I57" s="18"/>
+      <c r="J57" s="18"/>
+      <c r="K57" s="18"/>
+      <c r="L57" s="18"/>
+      <c r="M57" s="18"/>
+      <c r="N57" s="18"/>
+      <c r="O57" s="18"/>
+      <c r="P57" s="18"/>
       <c r="Q57" s="3"/>
       <c r="R57" s="3"/>
       <c r="S57" s="3"/>
-      <c r="T57" s="15">
+      <c r="T57" s="19">
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="17:20">
+    <row r="58" spans="1:20">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="18"/>
+      <c r="I58" s="18"/>
+      <c r="J58" s="18"/>
+      <c r="K58" s="18"/>
+      <c r="L58" s="18"/>
+      <c r="M58" s="18"/>
+      <c r="N58" s="18"/>
+      <c r="O58" s="18"/>
+      <c r="P58" s="18"/>
       <c r="Q58" s="3"/>
       <c r="R58" s="3"/>
       <c r="S58" s="3"/>
-      <c r="T58" s="15">
+      <c r="T58" s="19">
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="17:20">
+    <row r="59" spans="1:20">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="18"/>
+      <c r="I59" s="18"/>
+      <c r="J59" s="18"/>
+      <c r="K59" s="18"/>
+      <c r="L59" s="18"/>
+      <c r="M59" s="18"/>
+      <c r="N59" s="18"/>
+      <c r="O59" s="18"/>
+      <c r="P59" s="18"/>
       <c r="Q59" s="3"/>
       <c r="R59" s="3"/>
       <c r="S59" s="3"/>
-      <c r="T59" s="15">
+      <c r="T59" s="19">
         <v>49</v>
       </c>
     </row>
-    <row r="60" spans="17:20">
+    <row r="60" spans="1:20">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="18"/>
+      <c r="J60" s="18"/>
+      <c r="K60" s="18"/>
+      <c r="L60" s="18"/>
+      <c r="M60" s="18"/>
+      <c r="N60" s="18"/>
+      <c r="O60" s="18"/>
+      <c r="P60" s="18"/>
       <c r="Q60" s="3"/>
       <c r="R60" s="3"/>
       <c r="S60" s="3"/>
-      <c r="T60" s="15">
+      <c r="T60" s="19">
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="17:20">
+    <row r="61" spans="1:20">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
+      <c r="J61" s="18"/>
+      <c r="K61" s="18"/>
+      <c r="L61" s="18"/>
+      <c r="M61" s="18"/>
+      <c r="N61" s="18"/>
+      <c r="O61" s="18"/>
+      <c r="P61" s="18"/>
       <c r="Q61" s="3"/>
       <c r="R61" s="3"/>
       <c r="S61" s="3"/>
-      <c r="T61" s="15">
+      <c r="T61" s="19">
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="17:20">
+    <row r="62" spans="1:20">
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="18"/>
+      <c r="I62" s="18"/>
+      <c r="J62" s="18"/>
+      <c r="K62" s="18"/>
+      <c r="L62" s="18"/>
+      <c r="M62" s="18"/>
+      <c r="N62" s="18"/>
+      <c r="O62" s="18"/>
+      <c r="P62" s="18"/>
       <c r="Q62" s="3"/>
       <c r="R62" s="3"/>
       <c r="S62" s="3"/>
-      <c r="T62" s="15">
+      <c r="T62" s="19">
         <v>52</v>
       </c>
     </row>
-    <row r="63" spans="17:20">
+    <row r="63" spans="1:20">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="18"/>
+      <c r="I63" s="18"/>
+      <c r="J63" s="18"/>
+      <c r="K63" s="18"/>
+      <c r="L63" s="18"/>
+      <c r="M63" s="18"/>
+      <c r="N63" s="18"/>
+      <c r="O63" s="18"/>
+      <c r="P63" s="18"/>
       <c r="Q63" s="3"/>
       <c r="R63" s="3"/>
       <c r="S63" s="3"/>
-      <c r="T63" s="15">
+      <c r="T63" s="19">
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="20:20">
-      <c r="T64" s="15">
+    <row r="64" spans="1:20">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="18"/>
+      <c r="I64" s="18"/>
+      <c r="J64" s="18"/>
+      <c r="K64" s="18"/>
+      <c r="L64" s="18"/>
+      <c r="M64" s="18"/>
+      <c r="N64" s="18"/>
+      <c r="O64" s="18"/>
+      <c r="P64" s="18"/>
+      <c r="Q64" s="3"/>
+      <c r="R64" s="3"/>
+      <c r="S64" s="3"/>
+      <c r="T64" s="19">
         <v>54</v>
       </c>
     </row>
-    <row r="65" spans="20:20">
-      <c r="T65" s="15">
+    <row r="65" spans="1:20">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="18"/>
+      <c r="I65" s="18"/>
+      <c r="J65" s="18"/>
+      <c r="K65" s="18"/>
+      <c r="L65" s="18"/>
+      <c r="M65" s="18"/>
+      <c r="N65" s="18"/>
+      <c r="O65" s="18"/>
+      <c r="P65" s="18"/>
+      <c r="Q65" s="3"/>
+      <c r="R65" s="3"/>
+      <c r="S65" s="3"/>
+      <c r="T65" s="19">
         <v>55</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="133">
+  <mergeCells count="169">
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C10:P10"/>
     <mergeCell ref="Q10:S10"/>
@@ -2657,35 +3041,71 @@
     <mergeCell ref="C43:P43"/>
     <mergeCell ref="Q43:S43"/>
     <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C44:P44"/>
     <mergeCell ref="Q44:S44"/>
     <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C45:P45"/>
     <mergeCell ref="Q45:S45"/>
     <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:P46"/>
     <mergeCell ref="Q46:S46"/>
     <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:P47"/>
     <mergeCell ref="Q47:S47"/>
     <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:P48"/>
     <mergeCell ref="Q48:S48"/>
     <mergeCell ref="A49:B49"/>
+    <mergeCell ref="C49:P49"/>
     <mergeCell ref="Q49:S49"/>
     <mergeCell ref="A50:B50"/>
+    <mergeCell ref="C50:P50"/>
     <mergeCell ref="Q50:S50"/>
     <mergeCell ref="A51:B51"/>
+    <mergeCell ref="C51:P51"/>
     <mergeCell ref="Q51:S51"/>
     <mergeCell ref="A52:B52"/>
+    <mergeCell ref="C52:P52"/>
     <mergeCell ref="Q52:S52"/>
     <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C53:P53"/>
     <mergeCell ref="Q53:S53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="C54:P54"/>
     <mergeCell ref="Q54:S54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:P55"/>
     <mergeCell ref="Q55:S55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="C56:P56"/>
     <mergeCell ref="Q56:S56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="C57:P57"/>
     <mergeCell ref="Q57:S57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="C58:P58"/>
     <mergeCell ref="Q58:S58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="C59:P59"/>
     <mergeCell ref="Q59:S59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="C60:P60"/>
     <mergeCell ref="Q60:S60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="C61:P61"/>
     <mergeCell ref="Q61:S61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="C62:P62"/>
     <mergeCell ref="Q62:S62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="C63:P63"/>
     <mergeCell ref="Q63:S63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="C64:P64"/>
+    <mergeCell ref="Q64:S64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="C65:P65"/>
+    <mergeCell ref="Q65:S65"/>
     <mergeCell ref="A1:S5"/>
     <mergeCell ref="A7:S8"/>
   </mergeCells>
@@ -2723,6 +3143,10 @@
     <hyperlink ref="C42" r:id="rId31" display="https://codeforces.com/contest/1638/problem/B"/>
     <hyperlink ref="C43" r:id="rId32" display="https://codeforces.com/problemset/problem/1430/C"/>
     <hyperlink ref="C38" r:id="rId33" display="https://codeforces.com/contest/139/problem/A"/>
+    <hyperlink ref="C44:P44" r:id="rId33" display="https://codeforces.com/contest/139/problem/A"/>
+    <hyperlink ref="C45:P45" r:id="rId34" display="https://codeforces.com/problemset/problem/219/A"/>
+    <hyperlink ref="C46:P46" r:id="rId35" display="https://codeforces.com/problemset/problem/1141/A"/>
+    <hyperlink ref="C47:P47" r:id="rId36" display="https://codeforces.com/problemset/problem/118/B"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>